<commit_message>
Updates to Pneumo65, Mening schedules.  New Influenza diagram.
</commit_message>
<xml_diff>
--- a/schedules/Mening.xlsx
+++ b/schedules/Mening.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\forecast\forecaster2012\schedules\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="396"/>
   </bookViews>
@@ -17,14 +12,14 @@
   </sheets>
   <definedNames>
     <definedName name="Excel_BuiltIn_Print_Area_1">Schedules!$A$1:$K$44</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$K$104</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$K$103</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="65">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -276,8 +271,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -602,10 +597,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -629,7 +624,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:blipFill dpi="0" rotWithShape="0">
                 <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
                 <a:srcRect/>
@@ -640,7 +635,7 @@
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -650,7 +645,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -709,7 +704,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -744,7 +739,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -933,11 +928,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -947,7 +942,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -975,11 +970,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -989,7 +984,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1006,21 +1001,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
     <col min="2" max="3" width="14.42578125" style="1" customWidth="1"/>
@@ -1037,8 +1032,8 @@
     <col min="25" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10" ht="8.25" customHeight="1"/>
+    <row r="2" spans="2:10">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1054,7 +1049,7 @@
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1074,7 +1069,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10">
       <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1092,7 +1087,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10">
       <c r="B5" s="9" t="s">
         <v>10</v>
       </c>
@@ -1112,7 +1107,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10">
       <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
@@ -1132,7 +1127,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10">
       <c r="B7" s="9" t="s">
         <v>55</v>
       </c>
@@ -1150,7 +1145,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10">
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
@@ -1166,67 +1161,67 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10">
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10">
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10">
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10">
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10">
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10">
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10">
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10">
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9">
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9">
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9">
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9">
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9">
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9">
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9">
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="2:9" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9" ht="14.25">
       <c r="B24" s="5" t="s">
         <v>15</v>
       </c>
@@ -1240,7 +1235,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9">
       <c r="B25" s="15" t="s">
         <v>20</v>
       </c>
@@ -1251,7 +1246,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9">
       <c r="B26" s="22" t="s">
         <v>23</v>
       </c>
@@ -1259,7 +1254,7 @@
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9">
       <c r="B27" s="16"/>
       <c r="C27" s="6" t="s">
         <v>24</v>
@@ -1271,7 +1266,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:9">
       <c r="B28" s="17" t="s">
         <v>27</v>
       </c>
@@ -1285,7 +1280,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:9">
       <c r="B29" s="17" t="s">
         <v>31</v>
       </c>
@@ -1293,7 +1288,7 @@
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9">
       <c r="B30" s="17" t="s">
         <v>32</v>
       </c>
@@ -1303,7 +1298,7 @@
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:9">
       <c r="B31" s="17" t="s">
         <v>33</v>
       </c>
@@ -1313,7 +1308,7 @@
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9">
       <c r="B32" s="17" t="s">
         <v>35</v>
       </c>
@@ -1323,7 +1318,7 @@
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5">
       <c r="B33" s="17" t="s">
         <v>36</v>
       </c>
@@ -1333,7 +1328,7 @@
       </c>
       <c r="E33" s="9"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5">
       <c r="B34" s="17" t="s">
         <v>38</v>
       </c>
@@ -1341,14 +1336,14 @@
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5">
       <c r="B35" s="22" t="s">
         <v>39</v>
       </c>
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5">
       <c r="B36" s="6" t="s">
         <v>4</v>
       </c>
@@ -1362,7 +1357,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5">
       <c r="B37" s="9" t="s">
         <v>55</v>
       </c>
@@ -1376,7 +1371,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5">
       <c r="B38" s="9" t="s">
         <v>10</v>
       </c>
@@ -1390,7 +1385,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:5">
       <c r="B39" s="9" t="s">
         <v>7</v>
       </c>
@@ -1404,7 +1399,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:5">
       <c r="B40" s="9" t="s">
         <v>10</v>
       </c>
@@ -1414,7 +1409,7 @@
       <c r="D40" s="9"/>
       <c r="E40" s="19"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5">
       <c r="B41" s="9" t="s">
         <v>7</v>
       </c>
@@ -1426,7 +1421,7 @@
       </c>
       <c r="E41" s="19"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:5">
       <c r="B42" s="9" t="s">
         <v>7</v>
       </c>
@@ -1438,7 +1433,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:5">
       <c r="B43" s="17" t="s">
         <v>48</v>
       </c>
@@ -1446,7 +1441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:5">
       <c r="B44" s="17" t="s">
         <v>49</v>
       </c>
@@ -1454,7 +1449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:5" ht="14.25">
       <c r="B46" s="5" t="s">
         <v>15</v>
       </c>
@@ -1468,7 +1463,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:5">
       <c r="B47" s="15" t="s">
         <v>44</v>
       </c>
@@ -1477,7 +1472,7 @@
       </c>
       <c r="D47" s="15"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:5">
       <c r="B48" s="22" t="s">
         <v>23</v>
       </c>
@@ -1485,7 +1480,7 @@
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:5">
       <c r="B49" s="16"/>
       <c r="C49" s="6" t="s">
         <v>24</v>
@@ -1497,7 +1492,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:5">
       <c r="B50" s="17" t="s">
         <v>27</v>
       </c>
@@ -1509,7 +1504,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:5">
       <c r="B51" s="17" t="s">
         <v>31</v>
       </c>
@@ -1517,7 +1512,7 @@
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:5">
       <c r="B52" s="17" t="s">
         <v>32</v>
       </c>
@@ -1525,9 +1520,11 @@
         <v>43</v>
       </c>
       <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E52" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5">
       <c r="B53" s="17" t="s">
         <v>33</v>
       </c>
@@ -1537,7 +1534,7 @@
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:5">
       <c r="B54" s="17" t="s">
         <v>35</v>
       </c>
@@ -1547,7 +1544,7 @@
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:5">
       <c r="B55" s="17" t="s">
         <v>36</v>
       </c>
@@ -1559,7 +1556,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:5">
       <c r="B56" s="17" t="s">
         <v>38</v>
       </c>
@@ -1567,14 +1564,14 @@
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:5">
       <c r="B57" s="22" t="s">
         <v>39</v>
       </c>
       <c r="C57" s="22"/>
       <c r="D57" s="22"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:5">
       <c r="B58" s="6" t="s">
         <v>4</v>
       </c>
@@ -1588,7 +1585,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:5">
       <c r="B59" s="9" t="s">
         <v>55</v>
       </c>
@@ -1600,7 +1597,7 @@
       </c>
       <c r="E59" s="19"/>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:5">
       <c r="B60" s="9" t="s">
         <v>10</v>
       </c>
@@ -1610,7 +1607,7 @@
       <c r="D60" s="9"/>
       <c r="E60" s="19"/>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:5">
       <c r="B61" s="9" t="s">
         <v>7</v>
       </c>
@@ -1622,7 +1619,7 @@
       </c>
       <c r="E61" s="19"/>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:5">
       <c r="B62" s="9" t="s">
         <v>7</v>
       </c>
@@ -1632,7 +1629,7 @@
       <c r="D62" s="9"/>
       <c r="E62" s="19"/>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:5">
       <c r="B63" s="17" t="s">
         <v>48</v>
       </c>
@@ -1640,7 +1637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:5">
       <c r="B64" s="17" t="s">
         <v>49</v>
       </c>
@@ -1648,7 +1645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:5" ht="14.25">
       <c r="B66" s="5" t="s">
         <v>15</v>
       </c>
@@ -1660,7 +1657,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:5">
       <c r="B67" s="15" t="s">
         <v>42</v>
       </c>
@@ -1668,7 +1665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:5">
       <c r="B68" s="22" t="s">
         <v>23</v>
       </c>
@@ -1676,7 +1673,7 @@
       <c r="D68" s="22"/>
       <c r="E68" s="22"/>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:5">
       <c r="B69" s="16"/>
       <c r="C69" s="6" t="s">
         <v>24</v>
@@ -1688,7 +1685,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:5">
       <c r="B70" s="17" t="s">
         <v>27</v>
       </c>
@@ -1700,7 +1697,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:5">
       <c r="B71" s="17" t="s">
         <v>31</v>
       </c>
@@ -1708,7 +1705,7 @@
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
     </row>
-    <row r="72" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:5" ht="12" customHeight="1">
       <c r="B72" s="17" t="s">
         <v>32</v>
       </c>
@@ -1716,9 +1713,11 @@
         <v>43</v>
       </c>
       <c r="D72" s="9"/>
-      <c r="E72" s="9"/>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E72" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5">
       <c r="B73" s="17" t="s">
         <v>33</v>
       </c>
@@ -1728,7 +1727,7 @@
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:5">
       <c r="B74" s="17" t="s">
         <v>35</v>
       </c>
@@ -1738,7 +1737,7 @@
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:5">
       <c r="B75" s="17" t="s">
         <v>36</v>
       </c>
@@ -1750,7 +1749,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:5">
       <c r="B76" s="17" t="s">
         <v>38</v>
       </c>
@@ -1758,14 +1757,14 @@
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:5">
       <c r="B77" s="22" t="s">
         <v>39</v>
       </c>
       <c r="C77" s="22"/>
       <c r="D77" s="22"/>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:5">
       <c r="B78" s="6" t="s">
         <v>4</v>
       </c>
@@ -1779,7 +1778,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:5">
       <c r="B79" s="9" t="s">
         <v>55</v>
       </c>
@@ -1791,7 +1790,7 @@
       </c>
       <c r="E79" s="19"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:5">
       <c r="B80" s="9" t="s">
         <v>7</v>
       </c>
@@ -1801,7 +1800,7 @@
       <c r="D80" s="9"/>
       <c r="E80" s="19"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:5">
       <c r="B81" s="9" t="s">
         <v>10</v>
       </c>
@@ -1811,7 +1810,7 @@
       <c r="D81" s="9"/>
       <c r="E81" s="19"/>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:5">
       <c r="B82" s="17" t="s">
         <v>48</v>
       </c>
@@ -1819,7 +1818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:5">
       <c r="B83" s="17" t="s">
         <v>49</v>
       </c>
@@ -1827,7 +1826,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:5" ht="14.25">
       <c r="B85" s="5" t="s">
         <v>15</v>
       </c>
@@ -1839,7 +1838,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:5">
       <c r="B86" s="15" t="s">
         <v>22</v>
       </c>
@@ -1847,7 +1846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:5">
       <c r="B87" s="22" t="s">
         <v>23</v>
       </c>
@@ -1855,7 +1854,7 @@
       <c r="D87" s="22"/>
       <c r="E87" s="22"/>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:5">
       <c r="B88" s="16"/>
       <c r="C88" s="6" t="s">
         <v>24</v>
@@ -1867,7 +1866,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:5">
       <c r="B89" s="17" t="s">
         <v>27</v>
       </c>
@@ -1879,7 +1878,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:5">
       <c r="B90" s="17" t="s">
         <v>31</v>
       </c>
@@ -1887,7 +1886,7 @@
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:5">
       <c r="B91" s="17" t="s">
         <v>32</v>
       </c>
@@ -1897,7 +1896,7 @@
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:5">
       <c r="B92" s="17" t="s">
         <v>33</v>
       </c>
@@ -1907,7 +1906,7 @@
       <c r="D92" s="9"/>
       <c r="E92" s="9"/>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:5">
       <c r="B93" s="17" t="s">
         <v>35</v>
       </c>
@@ -1917,7 +1916,7 @@
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:5">
       <c r="B94" s="17" t="s">
         <v>36</v>
       </c>
@@ -1929,7 +1928,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:5">
       <c r="B95" s="17" t="s">
         <v>38</v>
       </c>
@@ -1937,14 +1936,14 @@
       <c r="D95" s="9"/>
       <c r="E95" s="9"/>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:5">
       <c r="B96" s="22" t="s">
         <v>39</v>
       </c>
       <c r="C96" s="22"/>
       <c r="D96" s="22"/>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:5">
       <c r="B97" s="6" t="s">
         <v>4</v>
       </c>
@@ -1958,7 +1957,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:5">
       <c r="B98" s="9" t="s">
         <v>7</v>
       </c>
@@ -1970,7 +1969,7 @@
       </c>
       <c r="E98" s="19"/>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:5">
       <c r="B99" s="9" t="s">
         <v>7</v>
       </c>
@@ -1980,7 +1979,7 @@
       <c r="D99" s="9"/>
       <c r="E99" s="19"/>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:5">
       <c r="B100" s="9" t="s">
         <v>10</v>
       </c>
@@ -1990,7 +1989,7 @@
       <c r="D100" s="9"/>
       <c r="E100" s="19"/>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:5">
       <c r="B101" s="17" t="s">
         <v>48</v>
       </c>
@@ -1998,7 +1997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:5">
       <c r="B102" s="17" t="s">
         <v>49</v>
       </c>
@@ -2009,15 +2008,15 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="9">
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B87:E87"/>
+    <mergeCell ref="B35:D35"/>
     <mergeCell ref="B96:D96"/>
     <mergeCell ref="B48:E48"/>
     <mergeCell ref="B68:E68"/>
     <mergeCell ref="B57:D57"/>
     <mergeCell ref="B77:D77"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B87:E87"/>
-    <mergeCell ref="B35:D35"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2034,385 +2033,383 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A62"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="106.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="20" t="str">
         <f>"&lt;forecast seriesName="&amp;CHAR(34)&amp;Schedules!D2&amp;CHAR(34)&amp;"&gt;"</f>
         <v>&lt;forecast seriesName="Mening"&gt;</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="MCV4" vaccineIds="183, 184, 198"/&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B5&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C5&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="MPSV4" vaccineIds="182"/&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B6&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C6&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Menveo" vaccineIds="198"/&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B7&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C7&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Menactra" vaccineIds="183"/&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1">
       <c r="A6" s="21" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B25&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C25&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D25&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E24&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="A1" dose="1" indication="BIRTH" label="1st"&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1">
       <c r="A7" s="20" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C44&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C43&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="1"/&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1">
       <c r="A8" s="21" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C28&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D28&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E28&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 weeks" interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1">
       <c r="A9" s="21" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C29&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D29&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E29&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1">
       <c r="A10" s="21" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C30&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D30&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E30&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="11 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1">
       <c r="A11" s="21" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C31&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D31&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E31&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="13 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1">
       <c r="A12" s="21" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C32&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D32&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E32&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="19 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1">
       <c r="A13" s="21" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D33&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E33&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1">
       <c r="A14" s="21" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D34&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1">
       <c r="A15" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B37&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C37&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D37&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E37&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Menactra" schedule="INVALID" age="9 months -4 days" reason="Menactra not licensed before 9 months."/&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1">
       <c r="A16" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B38&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C38&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D38&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E38&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="INVALID" age="2 years" reason="MPSV4 not licensed before 2 years."/&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B39&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C39&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D39&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E39&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="A1" age="10 years" reason="Received dose of MCV4 before 10 years, not counting towards completion."/&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B40&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C40&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D40&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E40&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="B1" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B41&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C41&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D41&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E41&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="A2" age="16 years" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B42&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C42&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D42&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E42&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="COMPLETE" age="" reason="Only one dose needed if administered after 15 years of age."/&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" s="21" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22" s="21" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B47&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C47&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D47&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E46&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="A2" dose="2" indication="" label="2nd"&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23" s="20" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C64&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C63&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1">
       <c r="A24" s="21" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C50&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D50&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E50&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1">
       <c r="A25" s="21" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C51&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D51&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E51&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1">
       <c r="A26" s="21" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C52&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D52&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E52&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;due age="16 years" interval="" grace=""/&gt;</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+        <v xml:space="preserve">    &lt;due age="16 years" interval="" grace="4 days"/&gt;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
       <c r="A27" s="21" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C53&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D53&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E53&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="17 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1">
       <c r="A28" s="21" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C54&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D54&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E54&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="19 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1">
       <c r="A29" s="21" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D55&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E55&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1">
       <c r="A30" s="21" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D56&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1">
       <c r="A31" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B59&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C59&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D59&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E59&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Menactra" schedule="INVALID" age="9 months" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1">
       <c r="A32" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B60&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C60&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D60&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E60&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="B1" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1">
       <c r="A33" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B61&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C61&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D61&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E61&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="B2" age="16 years" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B62&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C62&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D62&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E62&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1">
       <c r="A35" s="21" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1">
       <c r="A36" s="21" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B86&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C86&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D86&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E85&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="B1" dose="2" indication="" label="2nd after MPSV4"&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1">
       <c r="A37" s="20" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C102&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C101&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="2" column="1"/&gt;</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1">
       <c r="A38" s="21" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C89&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D89&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E89&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="5 years" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1">
       <c r="A39" s="21" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C90&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D90&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E90&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1">
       <c r="A40" s="21" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C91&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D91&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E91&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="11 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1">
       <c r="A41" s="21" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C92&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D92&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E92&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="13 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1">
       <c r="A42" s="21" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C93&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D93&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E93&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="19 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1">
       <c r="A43" s="21" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D94&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E94&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1">
       <c r="A44" s="21" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D95&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1">
       <c r="A45" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B98&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C98&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D98&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E98&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="B2" age="16 years" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1">
       <c r="A46" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B99&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C99&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D99&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E99&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1">
       <c r="A47" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B100&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C100&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D100&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E100&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="INVALID" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1">
       <c r="A48" s="21" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1">
       <c r="A49" s="21" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B67&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C67&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D67&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E66&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="B2" dose="3" indication="" label="3rd"&gt;</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1">
       <c r="A50" s="20" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C83&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C82&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="2" column="2"/&gt;</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1">
       <c r="A51" s="21" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C70&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D70&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E70&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1">
       <c r="A52" s="21" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C71&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D71&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E71&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1">
       <c r="A53" s="21" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C72&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D72&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E72&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;due age="16 years" interval="" grace=""/&gt;</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+        <v xml:space="preserve">    &lt;due age="16 years" interval="" grace="4 days"/&gt;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
       <c r="A54" s="21" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C73&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D73&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E73&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="17 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1">
       <c r="A55" s="21" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C74&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D74&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E74&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="19 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1">
       <c r="A56" s="21" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D75&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E75&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1">
       <c r="A57" s="21" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D76&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1">
       <c r="A58" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B79&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C79&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D79&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E79&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Menactra" schedule="INVALID" age="9 months" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1">
       <c r="A59" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B80&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C80&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D80&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E80&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1">
       <c r="A60" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B81&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C81&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D81&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E81&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="INVALID" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1">
       <c r="A61" s="21" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1">
       <c r="A62" s="20" t="str">
         <f>"&lt;/forecast&gt;"</f>
         <v>&lt;/forecast&gt;</v>
@@ -2421,7 +2418,7 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0263888888888888" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Revert Mening schedule to previous version
</commit_message>
<xml_diff>
--- a/schedules/Mening.xlsx
+++ b/schedules/Mening.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\forecast\forecaster2012\schedules\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="13185" tabRatio="396"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="396"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
@@ -12,14 +17,14 @@
   </sheets>
   <definedNames>
     <definedName name="Excel_BuiltIn_Print_Area_1">Schedules!$A$1:$K$44</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$K$103</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$K$104</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="65">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -267,15 +272,12 @@
   <si>
     <t>19 years</t>
   </si>
-  <si>
-    <t>16 years -4 days</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -600,10 +602,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -627,7 +629,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:blipFill dpi="0" rotWithShape="0">
                 <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
                 <a:srcRect/>
@@ -638,7 +640,7 @@
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -648,7 +650,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -707,7 +709,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -742,7 +744,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -931,11 +933,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr val="090000"/>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr val="400000"/>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -945,7 +947,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -973,11 +975,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr val="090000"/>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr val="400000"/>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -987,7 +989,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1004,21 +1006,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
     <col min="2" max="3" width="14.42578125" style="1" customWidth="1"/>
@@ -1035,8 +1037,8 @@
     <col min="25" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="8.25" customHeight="1"/>
-    <row r="2" spans="2:10">
+    <row r="1" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1052,7 +1054,7 @@
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1072,7 +1074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1090,7 +1092,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
         <v>10</v>
       </c>
@@ -1110,7 +1112,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
@@ -1130,7 +1132,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
         <v>55</v>
       </c>
@@ -1148,7 +1150,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
@@ -1164,67 +1166,67 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="2:9">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="2:9" ht="14.25">
+    <row r="24" spans="2:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>15</v>
       </c>
@@ -1238,7 +1240,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="15" t="s">
         <v>20</v>
       </c>
@@ -1249,7 +1251,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="22" t="s">
         <v>23</v>
       </c>
@@ -1257,7 +1259,7 @@
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="16"/>
       <c r="C27" s="6" t="s">
         <v>24</v>
@@ -1269,7 +1271,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="17" t="s">
         <v>27</v>
       </c>
@@ -1283,7 +1285,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:9">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="17" t="s">
         <v>31</v>
       </c>
@@ -1291,7 +1293,7 @@
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="2:9">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="17" t="s">
         <v>32</v>
       </c>
@@ -1301,7 +1303,7 @@
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
     </row>
-    <row r="31" spans="2:9">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="17" t="s">
         <v>33</v>
       </c>
@@ -1311,7 +1313,7 @@
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="2:9">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="17" t="s">
         <v>35</v>
       </c>
@@ -1321,7 +1323,7 @@
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="17" t="s">
         <v>36</v>
       </c>
@@ -1331,7 +1333,7 @@
       </c>
       <c r="E33" s="9"/>
     </row>
-    <row r="34" spans="2:5">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="17" t="s">
         <v>38</v>
       </c>
@@ -1339,14 +1341,14 @@
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="22" t="s">
         <v>39</v>
       </c>
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
         <v>4</v>
       </c>
@@ -1360,7 +1362,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="9" t="s">
         <v>55</v>
       </c>
@@ -1374,7 +1376,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="2:5">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="9" t="s">
         <v>10</v>
       </c>
@@ -1388,7 +1390,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="2:5">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="9" t="s">
         <v>7</v>
       </c>
@@ -1402,7 +1404,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="2:5">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" s="9" t="s">
         <v>10</v>
       </c>
@@ -1412,7 +1414,7 @@
       <c r="D40" s="9"/>
       <c r="E40" s="19"/>
     </row>
-    <row r="41" spans="2:5">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" s="9" t="s">
         <v>7</v>
       </c>
@@ -1420,11 +1422,11 @@
         <v>44</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="E41" s="19"/>
     </row>
-    <row r="42" spans="2:5">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" s="9" t="s">
         <v>7</v>
       </c>
@@ -1436,7 +1438,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="2:5">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="17" t="s">
         <v>48</v>
       </c>
@@ -1444,7 +1446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:5">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" s="17" t="s">
         <v>49</v>
       </c>
@@ -1452,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:5" ht="14.25">
+    <row r="46" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B46" s="5" t="s">
         <v>15</v>
       </c>
@@ -1466,7 +1468,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="2:5">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" s="15" t="s">
         <v>44</v>
       </c>
@@ -1475,7 +1477,7 @@
       </c>
       <c r="D47" s="15"/>
     </row>
-    <row r="48" spans="2:5">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" s="22" t="s">
         <v>23</v>
       </c>
@@ -1483,7 +1485,7 @@
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
     </row>
-    <row r="49" spans="2:5">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" s="16"/>
       <c r="C49" s="6" t="s">
         <v>24</v>
@@ -1495,13 +1497,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="2:5">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C50" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="C50" s="9"/>
       <c r="D50" s="9" t="s">
         <v>52</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="2:5">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="17" t="s">
         <v>31</v>
       </c>
@@ -1517,7 +1517,7 @@
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
     </row>
-    <row r="52" spans="2:5">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" s="17" t="s">
         <v>32</v>
       </c>
@@ -1527,7 +1527,7 @@
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
     </row>
-    <row r="53" spans="2:5">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" s="17" t="s">
         <v>33</v>
       </c>
@@ -1537,7 +1537,7 @@
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
     </row>
-    <row r="54" spans="2:5">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" s="17" t="s">
         <v>35</v>
       </c>
@@ -1547,7 +1547,7 @@
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
     </row>
-    <row r="55" spans="2:5">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" s="17" t="s">
         <v>36</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="2:5">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" s="17" t="s">
         <v>38</v>
       </c>
@@ -1567,14 +1567,14 @@
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
     </row>
-    <row r="57" spans="2:5">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" s="22" t="s">
         <v>39</v>
       </c>
       <c r="C57" s="22"/>
       <c r="D57" s="22"/>
     </row>
-    <row r="58" spans="2:5">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" s="6" t="s">
         <v>4</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="2:5">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" s="9" t="s">
         <v>55</v>
       </c>
@@ -1600,7 +1600,7 @@
       </c>
       <c r="E59" s="19"/>
     </row>
-    <row r="60" spans="2:5">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" s="9" t="s">
         <v>10</v>
       </c>
@@ -1610,7 +1610,7 @@
       <c r="D60" s="9"/>
       <c r="E60" s="19"/>
     </row>
-    <row r="61" spans="2:5">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" s="9" t="s">
         <v>7</v>
       </c>
@@ -1618,11 +1618,11 @@
         <v>42</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="E61" s="19"/>
     </row>
-    <row r="62" spans="2:5">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" s="9" t="s">
         <v>7</v>
       </c>
@@ -1632,7 +1632,7 @@
       <c r="D62" s="9"/>
       <c r="E62" s="19"/>
     </row>
-    <row r="63" spans="2:5">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" s="17" t="s">
         <v>48</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="2:5">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" s="17" t="s">
         <v>49</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:5" ht="14.25">
+    <row r="66" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B66" s="5" t="s">
         <v>15</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="2:5">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B67" s="15" t="s">
         <v>42</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="2:5">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B68" s="22" t="s">
         <v>23</v>
       </c>
@@ -1676,7 +1676,7 @@
       <c r="D68" s="22"/>
       <c r="E68" s="22"/>
     </row>
-    <row r="69" spans="2:5">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B69" s="16"/>
       <c r="C69" s="6" t="s">
         <v>24</v>
@@ -1688,13 +1688,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="2:5">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B70" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C70" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="C70" s="9"/>
       <c r="D70" s="9" t="s">
         <v>52</v>
       </c>
@@ -1702,7 +1700,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="2:5">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B71" s="17" t="s">
         <v>31</v>
       </c>
@@ -1710,7 +1708,7 @@
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
     </row>
-    <row r="72" spans="2:5" ht="12" customHeight="1">
+    <row r="72" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="17" t="s">
         <v>32</v>
       </c>
@@ -1720,7 +1718,7 @@
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
     </row>
-    <row r="73" spans="2:5">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B73" s="17" t="s">
         <v>33</v>
       </c>
@@ -1730,7 +1728,7 @@
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
     </row>
-    <row r="74" spans="2:5">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B74" s="17" t="s">
         <v>35</v>
       </c>
@@ -1740,7 +1738,7 @@
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
     </row>
-    <row r="75" spans="2:5">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B75" s="17" t="s">
         <v>36</v>
       </c>
@@ -1752,7 +1750,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="2:5">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B76" s="17" t="s">
         <v>38</v>
       </c>
@@ -1760,14 +1758,14 @@
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
     </row>
-    <row r="77" spans="2:5">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B77" s="22" t="s">
         <v>39</v>
       </c>
       <c r="C77" s="22"/>
       <c r="D77" s="22"/>
     </row>
-    <row r="78" spans="2:5">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B78" s="6" t="s">
         <v>4</v>
       </c>
@@ -1781,7 +1779,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="79" spans="2:5">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B79" s="9" t="s">
         <v>55</v>
       </c>
@@ -1793,7 +1791,7 @@
       </c>
       <c r="E79" s="19"/>
     </row>
-    <row r="80" spans="2:5">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B80" s="9" t="s">
         <v>7</v>
       </c>
@@ -1803,7 +1801,7 @@
       <c r="D80" s="9"/>
       <c r="E80" s="19"/>
     </row>
-    <row r="81" spans="2:5">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B81" s="9" t="s">
         <v>10</v>
       </c>
@@ -1813,7 +1811,7 @@
       <c r="D81" s="9"/>
       <c r="E81" s="19"/>
     </row>
-    <row r="82" spans="2:5">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B82" s="17" t="s">
         <v>48</v>
       </c>
@@ -1821,7 +1819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="2:5">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B83" s="17" t="s">
         <v>49</v>
       </c>
@@ -1829,7 +1827,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="2:5" ht="14.25">
+    <row r="85" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B85" s="5" t="s">
         <v>15</v>
       </c>
@@ -1841,7 +1839,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="86" spans="2:5">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B86" s="15" t="s">
         <v>22</v>
       </c>
@@ -1849,7 +1847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="2:5">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B87" s="22" t="s">
         <v>23</v>
       </c>
@@ -1857,7 +1855,7 @@
       <c r="D87" s="22"/>
       <c r="E87" s="22"/>
     </row>
-    <row r="88" spans="2:5">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B88" s="16"/>
       <c r="C88" s="6" t="s">
         <v>24</v>
@@ -1869,7 +1867,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="2:5">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B89" s="17" t="s">
         <v>27</v>
       </c>
@@ -1881,7 +1879,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="2:5">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B90" s="17" t="s">
         <v>31</v>
       </c>
@@ -1889,7 +1887,7 @@
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
     </row>
-    <row r="91" spans="2:5">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B91" s="17" t="s">
         <v>32</v>
       </c>
@@ -1899,7 +1897,7 @@
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
     </row>
-    <row r="92" spans="2:5">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B92" s="17" t="s">
         <v>33</v>
       </c>
@@ -1909,7 +1907,7 @@
       <c r="D92" s="9"/>
       <c r="E92" s="9"/>
     </row>
-    <row r="93" spans="2:5">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B93" s="17" t="s">
         <v>35</v>
       </c>
@@ -1919,7 +1917,7 @@
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
     </row>
-    <row r="94" spans="2:5">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B94" s="17" t="s">
         <v>36</v>
       </c>
@@ -1931,7 +1929,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="95" spans="2:5">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B95" s="17" t="s">
         <v>38</v>
       </c>
@@ -1939,14 +1937,14 @@
       <c r="D95" s="9"/>
       <c r="E95" s="9"/>
     </row>
-    <row r="96" spans="2:5">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B96" s="22" t="s">
         <v>39</v>
       </c>
       <c r="C96" s="22"/>
       <c r="D96" s="22"/>
     </row>
-    <row r="97" spans="2:5">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B97" s="6" t="s">
         <v>4</v>
       </c>
@@ -1960,7 +1958,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="98" spans="2:5">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B98" s="9" t="s">
         <v>7</v>
       </c>
@@ -1972,7 +1970,7 @@
       </c>
       <c r="E98" s="19"/>
     </row>
-    <row r="99" spans="2:5">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B99" s="9" t="s">
         <v>7</v>
       </c>
@@ -1982,7 +1980,7 @@
       <c r="D99" s="9"/>
       <c r="E99" s="19"/>
     </row>
-    <row r="100" spans="2:5">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B100" s="9" t="s">
         <v>10</v>
       </c>
@@ -1992,7 +1990,7 @@
       <c r="D100" s="9"/>
       <c r="E100" s="19"/>
     </row>
-    <row r="101" spans="2:5">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B101" s="17" t="s">
         <v>48</v>
       </c>
@@ -2000,7 +1998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="2:5">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B102" s="17" t="s">
         <v>49</v>
       </c>
@@ -2011,15 +2009,15 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="9">
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B87:E87"/>
-    <mergeCell ref="B35:D35"/>
     <mergeCell ref="B96:D96"/>
     <mergeCell ref="B48:E48"/>
     <mergeCell ref="B68:E68"/>
     <mergeCell ref="B57:D57"/>
     <mergeCell ref="B77:D77"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B87:E87"/>
+    <mergeCell ref="B35:D35"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2036,385 +2034,385 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A62"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="106.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="str">
         <f>"&lt;forecast seriesName="&amp;CHAR(34)&amp;Schedules!D2&amp;CHAR(34)&amp;"&gt;"</f>
         <v>&lt;forecast seriesName="Mening"&gt;</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="MCV4" vaccineIds="183, 184, 198"/&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B5&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C5&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="MPSV4" vaccineIds="182"/&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B6&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C6&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Menveo" vaccineIds="198"/&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B7&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C7&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Menactra" vaccineIds="183"/&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B25&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C25&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D25&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E24&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="A1" dose="1" indication="BIRTH" label="1st"&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C44&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C43&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="1"/&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C28&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D28&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E28&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 weeks" interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C29&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D29&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E29&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C30&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D30&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E30&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="11 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C31&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D31&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E31&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="13 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C32&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D32&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E32&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="19 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D33&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E33&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D34&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B37&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C37&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D37&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E37&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Menactra" schedule="INVALID" age="9 months -4 days" reason="Menactra not licensed before 9 months."/&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B38&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C38&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D38&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E38&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="INVALID" age="2 years" reason="MPSV4 not licensed before 2 years."/&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B39&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C39&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D39&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E39&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="A1" age="10 years" reason="Received dose of MCV4 before 10 years, not counting towards completion."/&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B40&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C40&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D40&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E40&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="B1" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B41&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C41&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D41&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E41&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="A2" age="16 years -4 days" reason=""/&gt;</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
+        <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="A2" age="16 years" reason=""/&gt;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B42&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C42&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D42&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E42&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="COMPLETE" age="" reason="Only one dose needed if administered after 15 years of age."/&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="21" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="21" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B47&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C47&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D47&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E46&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="A2" dose="2" indication="" label="2nd"&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C64&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C63&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C50&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D50&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E50&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;valid age="16 years" interval="8 weeks" grace="4 days"/&gt;</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
+        <v xml:space="preserve">    &lt;valid age="" interval="8 weeks" grace="4 days"/&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C51&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D51&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E51&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C52&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D52&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E52&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="16 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C53&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D53&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E53&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="17 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C54&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D54&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E54&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="19 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D55&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E55&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D56&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B59&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C59&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D59&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E59&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Menactra" schedule="INVALID" age="9 months" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B60&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C60&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D60&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E60&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="B1" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B61&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C61&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D61&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E61&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="B2" age="16 years -4 days" reason=""/&gt;</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
+        <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="B2" age="16 years" reason=""/&gt;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B62&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C62&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D62&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E62&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B86&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C86&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D86&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E85&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="B1" dose="2" indication="" label="2nd after MPSV4"&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C102&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C101&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="2" column="1"/&gt;</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C89&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D89&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E89&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="5 years" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C90&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D90&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E90&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="21" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C91&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D91&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E91&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="11 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="21" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C92&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D92&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E92&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="13 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="21" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C93&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D93&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E93&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="19 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D94&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E94&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="21" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D95&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B98&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C98&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D98&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E98&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="B2" age="16 years" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B99&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C99&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D99&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E99&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B100&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C100&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D100&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E100&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="INVALID" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="21" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="21" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B67&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C67&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D67&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E66&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="B2" dose="3" indication="" label="3rd"&gt;</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C83&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C82&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="2" column="2"/&gt;</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="21" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C70&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D70&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E70&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;valid age="16 years" interval="8 weeks" grace="4 days"/&gt;</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
+        <v xml:space="preserve">    &lt;valid age="" interval="8 weeks" grace="4 days"/&gt;</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="21" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C71&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D71&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E71&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="21" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C72&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D72&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E72&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="16 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="21" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C73&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D73&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E73&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="17 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="21" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C74&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D74&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E74&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="19 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="21" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D75&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E75&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="21" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D76&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B79&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C79&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D79&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E79&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Menactra" schedule="INVALID" age="9 months" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B80&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C80&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D80&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E80&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B81&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C81&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D81&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E81&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="INVALID" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="21" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="20" t="str">
         <f>"&lt;/forecast&gt;"</f>
         <v>&lt;/forecast&gt;</v>
@@ -2423,7 +2421,7 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0263888888888888" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Brady updated the XML tab to capture all immunization information for the simplified schedule.
</commit_message>
<xml_diff>
--- a/schedules/Mening.xlsx
+++ b/schedules/Mening.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCHWorkspaceJava6\forecaster\schedules\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="396" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19335" windowHeight="18585" tabRatio="396"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
@@ -19,12 +14,12 @@
     <definedName name="Excel_BuiltIn_Print_Area_1">Schedules!$A$1:$K$47</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$K$70</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="62">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -199,9 +194,6 @@
     <t>Menactra</t>
   </si>
   <si>
-    <t>2 years</t>
-  </si>
-  <si>
     <t>Menactra not licensed before 9 months.</t>
   </si>
   <si>
@@ -214,12 +206,6 @@
     <t>Received dose of MCV4 before 10 years, not counting towards completion.</t>
   </si>
   <si>
-    <t>19 years</t>
-  </si>
-  <si>
-    <t>2 months</t>
-  </si>
-  <si>
     <t>Received dose of MPSV4 before 10 years, not counting towards completion.</t>
   </si>
   <si>
@@ -238,17 +224,20 @@
     <t>9 months -4 days</t>
   </si>
   <si>
-    <t xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="A2" age="16 years -4 days" reason="Received dose before 16 years of age, not counting towards completion."/&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="A2" age="16 years -4 days" reason="Received dose before 16 years of age, not counting towards completion."/&gt;</t>
+    <t>22 years</t>
+  </si>
+  <si>
+    <t>2 months -4 days</t>
+  </si>
+  <si>
+    <t>2 years -4 days</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -290,7 +279,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,12 +320,6 @@
       <patternFill patternType="solid">
         <fgColor indexed="44"/>
         <bgColor indexed="31"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFDF85"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -417,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -468,9 +451,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -594,10 +574,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -617,7 +597,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -674,7 +654,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -709,7 +689,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -898,11 +878,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -912,7 +892,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -940,11 +920,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -954,7 +934,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -971,21 +951,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:J67"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
     <col min="2" max="3" width="14.42578125" style="1" customWidth="1"/>
@@ -1002,8 +982,8 @@
     <col min="25" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10" ht="8.25" customHeight="1"/>
+    <row r="2" spans="2:10">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1011,15 +991,15 @@
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+    </row>
+    <row r="3" spans="2:10">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1039,7 +1019,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10">
       <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1057,7 +1037,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10">
       <c r="B5" s="9" t="s">
         <v>10</v>
       </c>
@@ -1077,7 +1057,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10">
       <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
@@ -1097,7 +1077,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10">
       <c r="B7" s="9" t="s">
         <v>48</v>
       </c>
@@ -1115,7 +1095,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10">
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
@@ -1131,67 +1111,67 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10">
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10">
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10">
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10">
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10">
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10">
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10">
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10">
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9">
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9">
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9">
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9">
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9">
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9">
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9">
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="2:9" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9" ht="14.25">
       <c r="B24" s="5" t="s">
         <v>15</v>
       </c>
@@ -1205,8 +1185,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="22" t="s">
+    <row r="25" spans="2:9">
+      <c r="B25" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="15">
@@ -1216,15 +1196,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="26" t="s">
+    <row r="26" spans="2:9">
+      <c r="B26" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+    </row>
+    <row r="27" spans="2:9">
       <c r="B27" s="16"/>
       <c r="C27" s="6" t="s">
         <v>22</v>
@@ -1236,7 +1216,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:9">
       <c r="B28" s="17" t="s">
         <v>25</v>
       </c>
@@ -1250,7 +1230,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:9">
       <c r="B29" s="17" t="s">
         <v>28</v>
       </c>
@@ -1258,7 +1238,7 @@
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9">
       <c r="B30" s="17" t="s">
         <v>29</v>
       </c>
@@ -1268,7 +1248,7 @@
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:9">
       <c r="B31" s="17" t="s">
         <v>30</v>
       </c>
@@ -1278,17 +1258,17 @@
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9">
       <c r="B32" s="17" t="s">
         <v>32</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5">
       <c r="B33" s="17" t="s">
         <v>33</v>
       </c>
@@ -1300,7 +1280,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5">
       <c r="B34" s="17" t="s">
         <v>34</v>
       </c>
@@ -1308,14 +1288,14 @@
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="26" t="s">
+    <row r="35" spans="2:5">
+      <c r="B35" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+    </row>
+    <row r="36" spans="2:5">
       <c r="B36" s="6" t="s">
         <v>4</v>
       </c>
@@ -1329,7 +1309,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5">
       <c r="B37" s="9" t="s">
         <v>48</v>
       </c>
@@ -1337,13 +1317,13 @@
         <v>42</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
       <c r="B38" s="9" t="s">
         <v>10</v>
       </c>
@@ -1351,13 +1331,13 @@
         <v>42</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5">
       <c r="B39" s="9" t="s">
         <v>14</v>
       </c>
@@ -1365,13 +1345,13 @@
         <v>42</v>
       </c>
       <c r="D39" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="2:5">
       <c r="B40" s="9" t="s">
         <v>7</v>
       </c>
@@ -1379,13 +1359,13 @@
         <v>19</v>
       </c>
       <c r="D40" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E40" s="19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="2:5">
       <c r="B41" s="9" t="s">
         <v>10</v>
       </c>
@@ -1393,13 +1373,13 @@
         <v>19</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E41" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5">
       <c r="B42" s="9" t="s">
         <v>7</v>
       </c>
@@ -1407,11 +1387,11 @@
         <v>39</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E42" s="19"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:5">
       <c r="B43" s="9" t="s">
         <v>10</v>
       </c>
@@ -1419,11 +1399,11 @@
         <v>39</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E43" s="19"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:5">
       <c r="B44" s="9" t="s">
         <v>7</v>
       </c>
@@ -1435,7 +1415,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:5">
       <c r="B45" s="9" t="s">
         <v>10</v>
       </c>
@@ -1447,7 +1427,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:5">
       <c r="B46" s="17" t="s">
         <v>43</v>
       </c>
@@ -1455,7 +1435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:5">
       <c r="B47" s="17" t="s">
         <v>44</v>
       </c>
@@ -1463,7 +1443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:5" ht="14.25">
       <c r="B49" s="5" t="s">
         <v>15</v>
       </c>
@@ -1477,7 +1457,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:5">
       <c r="B50" s="15" t="s">
         <v>39</v>
       </c>
@@ -1486,15 +1466,15 @@
       </c>
       <c r="D50" s="15"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B51" s="23" t="s">
+    <row r="51" spans="2:5">
+      <c r="B51" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="25"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="24"/>
+    </row>
+    <row r="52" spans="2:5">
       <c r="B52" s="16"/>
       <c r="C52" s="6" t="s">
         <v>22</v>
@@ -1506,7 +1486,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:5">
       <c r="B53" s="17" t="s">
         <v>25</v>
       </c>
@@ -1520,7 +1500,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:5">
       <c r="B54" s="17" t="s">
         <v>28</v>
       </c>
@@ -1528,7 +1508,7 @@
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:5">
       <c r="B55" s="17" t="s">
         <v>29</v>
       </c>
@@ -1538,7 +1518,7 @@
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:5">
       <c r="B56" s="17" t="s">
         <v>30</v>
       </c>
@@ -1548,17 +1528,17 @@
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:5">
       <c r="B57" s="17" t="s">
         <v>32</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:5">
       <c r="B58" s="17" t="s">
         <v>33</v>
       </c>
@@ -1570,7 +1550,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:5">
       <c r="B59" s="17" t="s">
         <v>34</v>
       </c>
@@ -1578,14 +1558,14 @@
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B60" s="23" t="s">
+    <row r="60" spans="2:5">
+      <c r="B60" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C60" s="24"/>
-      <c r="D60" s="25"/>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C60" s="23"/>
+      <c r="D60" s="24"/>
+    </row>
+    <row r="61" spans="2:5">
       <c r="B61" s="6" t="s">
         <v>4</v>
       </c>
@@ -1599,7 +1579,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:5">
       <c r="B62" s="9" t="s">
         <v>7</v>
       </c>
@@ -1607,13 +1587,13 @@
         <v>39</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E62" s="19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5">
       <c r="B63" s="9" t="s">
         <v>10</v>
       </c>
@@ -1621,13 +1601,13 @@
         <v>39</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E63" s="19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5">
       <c r="B64" s="9" t="s">
         <v>7</v>
       </c>
@@ -1637,7 +1617,7 @@
       <c r="D64" s="9"/>
       <c r="E64" s="19"/>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:5">
       <c r="B65" s="9" t="s">
         <v>10</v>
       </c>
@@ -1647,7 +1627,7 @@
       <c r="D65" s="9"/>
       <c r="E65" s="19"/>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:5">
       <c r="B66" s="17" t="s">
         <v>43</v>
       </c>
@@ -1655,7 +1635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:5">
       <c r="B67" s="17" t="s">
         <v>44</v>
       </c>
@@ -1687,308 +1667,328 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection sqref="A1:A36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="145.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="20" t="str">
         <f>"&lt;forecast seriesName="&amp;CHAR(34)&amp;Schedules!D2&amp;CHAR(34)&amp;"&gt;"</f>
         <v>&lt;forecast seriesName="Mening"&gt;</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="MCV4" vaccineIds="183, 184, 198"/&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B5&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C5&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="MPSV4" vaccineIds="182"/&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B6&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C6&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Menveo" vaccineIds="198"/&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B7&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C7&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Menactra" vaccineIds="183"/&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1">
       <c r="A6" s="21" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B25&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C25&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D25&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E24&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="A1" dose="1" indication="BIRTH" label="1st"&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1">
       <c r="A7" s="20" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C47&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C46&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="1"/&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1">
       <c r="A8" s="21" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C28&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D28&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E28&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="8 weeks" interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1">
       <c r="A9" s="21" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C29&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D29&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E29&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1">
       <c r="A10" s="21" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C30&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D30&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E30&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="11 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1">
       <c r="A11" s="21" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C31&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D31&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E31&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="13 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1">
       <c r="A12" s="21" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C32&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D32&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E32&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;finished age="19 years" interval="" grace=""/&gt;</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+        <v xml:space="preserve">    &lt;finished age="22 years" interval="" grace=""/&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
       <c r="A13" s="21" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D33&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E33&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1">
       <c r="A14" s="21" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D34&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1">
       <c r="A15" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B37&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C37&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D37&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E37&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Menactra" schedule="INVALID" age="9 months -4 days" reason="Menactra not licensed before 9 months."/&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1">
       <c r="A16" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B38&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C38&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D38&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E38&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="INVALID" age="2 years" reason="MPSV4 not licensed before 2 years."/&gt;</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+        <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="INVALID" age="2 years -4 days" reason="MPSV4 not licensed before 2 years."/&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
       <c r="A17" s="21" t="str">
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B39&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C39&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D39&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E39&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;indicate vaccineName="Menveo" schedule="INVALID" age="2 months -4 days" reason="Menveo not licensed before 2 months."/&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B40&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C40&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D40&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E40&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="A1" age="10 years" reason="Received dose of MCV4 before 10 years, not counting towards completion."/&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="21" t="str">
+    <row r="19" spans="1:1">
+      <c r="A19" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B41&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C41&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D41&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E41&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="A1" age="10 years" reason="Received dose of MPSV4 before 10 years, not counting towards completion."/&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="21" t="str">
+    <row r="20" spans="1:1">
+      <c r="A20" s="21" t="str">
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B42&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C42&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D42&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E42&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="A2" age="16 years -4 days" reason=""/&gt;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B43&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C43&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D43&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E43&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="A2" age="16 years -4 days" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="str">
+    <row r="22" spans="1:1">
+      <c r="A22" s="21" t="str">
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B44&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C44&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D44&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E44&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="COMPLETE" age="" reason="Only one dose needed if administered after 15 years of age."/&gt;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B45&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C45&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D45&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E45&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="COMPLETE" age="" reason="Only one dose needed if administered after 15 years of age."/&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="21" t="str">
+    <row r="24" spans="1:1">
+      <c r="A24" s="21" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="21" t="str">
+    <row r="25" spans="1:1">
+      <c r="A25" s="21" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B50&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C50&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D50&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E49&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="A2" dose="2" indication="" label="2nd"&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="20" t="str">
+    <row r="26" spans="1:1">
+      <c r="A26" s="20" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C67&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C66&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="21" t="str">
+    <row r="27" spans="1:1">
+      <c r="A27" s="21" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C53&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D53&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E53&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="16 years" interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="21" t="str">
+    <row r="28" spans="1:1">
+      <c r="A28" s="21" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C54&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D54&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E54&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="21" t="str">
+    <row r="29" spans="1:1">
+      <c r="A29" s="21" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C55&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D55&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E55&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="16 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="21" t="str">
+    <row r="30" spans="1:1">
+      <c r="A30" s="21" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C56&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D56&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E56&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="17 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="21" t="str">
+    <row r="31" spans="1:1">
+      <c r="A31" s="21" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C57&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D57&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E57&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;finished age="19 years" interval="" grace=""/&gt;</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="21" t="str">
+        <v xml:space="preserve">    &lt;finished age="22 years" interval="" grace=""/&gt;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="21" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D58&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E58&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="21" t="str">
+    <row r="33" spans="1:1">
+      <c r="A33" s="21" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D59&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="21" t="str">
+    <row r="34" spans="1:1">
+      <c r="A34" s="21" t="str">
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B62&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C62&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D62&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E62&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="A2" age="16 years -4 days" reason="Received dose before 16 years of age, not counting towards completion."/&gt;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="21" t="str">
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B63&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C63&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D63&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E63&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="A2" age="16 years -4 days" reason="Received dose before 16 years of age, not counting towards completion."/&gt;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B64&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C64&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D64&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E64&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="21" t="str">
+    <row r="37" spans="1:1">
+      <c r="A37" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B65&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C65&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D65&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E65&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="21" t="str">
+    <row r="38" spans="1:1">
+      <c r="A38" s="21" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="20"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="21"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="21"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="21"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1">
+      <c r="A39" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="20"/>
+    </row>
+    <row r="41" spans="1:1">
       <c r="A41" s="21"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1">
       <c r="A42" s="21"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1">
       <c r="A43" s="21"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1">
       <c r="A44" s="21"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1">
       <c r="A45" s="21"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1">
       <c r="A46" s="21"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1">
       <c r="A47" s="21"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1">
       <c r="A48" s="21"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1">
       <c r="A49" s="21"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="20"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1">
+      <c r="A50" s="21"/>
+    </row>
+    <row r="51" spans="1:1">
       <c r="A51" s="21"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1">
       <c r="A52" s="21"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="21"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1">
+      <c r="A53" s="20"/>
+    </row>
+    <row r="54" spans="1:1">
       <c r="A54" s="21"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1">
       <c r="A55" s="21"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1">
       <c r="A56" s="21"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1">
       <c r="A57" s="21"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1">
       <c r="A58" s="21"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1">
       <c r="A59" s="21"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1">
       <c r="A60" s="21"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1">
       <c r="A61" s="21"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="20"/>
+    <row r="62" spans="1:1">
+      <c r="A62" s="21"/>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="21"/>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="21"/>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="20"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Change Finished Age from 22 to 19 years old.
</commit_message>
<xml_diff>
--- a/schedules/Mening.xlsx
+++ b/schedules/Mening.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCHWorkspaceJava6\forecaster\schedules\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19335" windowHeight="18585" tabRatio="396"/>
+    <workbookView xWindow="1380" yWindow="0" windowWidth="19335" windowHeight="18585" tabRatio="396"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
@@ -14,12 +19,12 @@
     <definedName name="Excel_BuiltIn_Print_Area_1">Schedules!$A$1:$K$47</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$K$70</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="63">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -232,12 +237,15 @@
   <si>
     <t>2 years -4 days</t>
   </si>
+  <si>
+    <t>19 years</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -577,7 +585,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -597,7 +605,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -892,7 +900,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -934,7 +942,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -951,21 +959,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
     <col min="2" max="3" width="14.42578125" style="1" customWidth="1"/>
@@ -982,8 +990,8 @@
     <col min="25" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="8.25" customHeight="1"/>
-    <row r="2" spans="2:10">
+    <row r="1" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -999,7 +1007,7 @@
       <c r="I2" s="25"/>
       <c r="J2" s="25"/>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1019,7 +1027,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1037,7 +1045,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
         <v>10</v>
       </c>
@@ -1057,7 +1065,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
@@ -1077,7 +1085,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
         <v>48</v>
       </c>
@@ -1095,7 +1103,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
@@ -1111,67 +1119,67 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="2:9">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="2:9" ht="14.25">
+    <row r="24" spans="2:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>15</v>
       </c>
@@ -1185,7 +1193,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="15" t="s">
         <v>19</v>
       </c>
@@ -1196,7 +1204,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="25" t="s">
         <v>21</v>
       </c>
@@ -1204,7 +1212,7 @@
       <c r="D26" s="25"/>
       <c r="E26" s="25"/>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="16"/>
       <c r="C27" s="6" t="s">
         <v>22</v>
@@ -1216,7 +1224,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="17" t="s">
         <v>25</v>
       </c>
@@ -1230,7 +1238,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:9">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="17" t="s">
         <v>28</v>
       </c>
@@ -1238,7 +1246,7 @@
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="2:9">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="17" t="s">
         <v>29</v>
       </c>
@@ -1248,7 +1256,7 @@
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
     </row>
-    <row r="31" spans="2:9">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="17" t="s">
         <v>30</v>
       </c>
@@ -1258,7 +1266,7 @@
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="2:9">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="17" t="s">
         <v>32</v>
       </c>
@@ -1268,7 +1276,7 @@
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="17" t="s">
         <v>33</v>
       </c>
@@ -1280,7 +1288,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="2:5">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="17" t="s">
         <v>34</v>
       </c>
@@ -1288,14 +1296,14 @@
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C35" s="25"/>
       <c r="D35" s="25"/>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
         <v>4</v>
       </c>
@@ -1309,7 +1317,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="9" t="s">
         <v>48</v>
       </c>
@@ -1323,7 +1331,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="2:5">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="9" t="s">
         <v>10</v>
       </c>
@@ -1337,7 +1345,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="2:5">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="9" t="s">
         <v>14</v>
       </c>
@@ -1351,7 +1359,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="2:5">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" s="9" t="s">
         <v>7</v>
       </c>
@@ -1365,7 +1373,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="2:5">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" s="9" t="s">
         <v>10</v>
       </c>
@@ -1379,7 +1387,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="2:5">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" s="9" t="s">
         <v>7</v>
       </c>
@@ -1391,7 +1399,7 @@
       </c>
       <c r="E42" s="19"/>
     </row>
-    <row r="43" spans="2:5">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="9" t="s">
         <v>10</v>
       </c>
@@ -1403,7 +1411,7 @@
       </c>
       <c r="E43" s="19"/>
     </row>
-    <row r="44" spans="2:5">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" s="9" t="s">
         <v>7</v>
       </c>
@@ -1415,7 +1423,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="2:5">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" s="9" t="s">
         <v>10</v>
       </c>
@@ -1427,7 +1435,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="2:5">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" s="17" t="s">
         <v>43</v>
       </c>
@@ -1435,7 +1443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:5">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" s="17" t="s">
         <v>44</v>
       </c>
@@ -1443,7 +1451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:5" ht="14.25">
+    <row r="49" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B49" s="5" t="s">
         <v>15</v>
       </c>
@@ -1457,7 +1465,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="2:5">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" s="15" t="s">
         <v>39</v>
       </c>
@@ -1466,7 +1474,7 @@
       </c>
       <c r="D50" s="15"/>
     </row>
-    <row r="51" spans="2:5">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="22" t="s">
         <v>21</v>
       </c>
@@ -1474,7 +1482,7 @@
       <c r="D51" s="23"/>
       <c r="E51" s="24"/>
     </row>
-    <row r="52" spans="2:5">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" s="16"/>
       <c r="C52" s="6" t="s">
         <v>22</v>
@@ -1486,7 +1494,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="2:5">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" s="17" t="s">
         <v>25</v>
       </c>
@@ -1500,7 +1508,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="2:5">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" s="17" t="s">
         <v>28</v>
       </c>
@@ -1508,7 +1516,7 @@
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
     </row>
-    <row r="55" spans="2:5">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" s="17" t="s">
         <v>29</v>
       </c>
@@ -1518,7 +1526,7 @@
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
     </row>
-    <row r="56" spans="2:5">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" s="17" t="s">
         <v>30</v>
       </c>
@@ -1528,17 +1536,17 @@
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
     </row>
-    <row r="57" spans="2:5">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" s="17" t="s">
         <v>32</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
     </row>
-    <row r="58" spans="2:5">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" s="17" t="s">
         <v>33</v>
       </c>
@@ -1550,7 +1558,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="2:5">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" s="17" t="s">
         <v>34</v>
       </c>
@@ -1558,14 +1566,14 @@
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
     </row>
-    <row r="60" spans="2:5">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" s="22" t="s">
         <v>35</v>
       </c>
       <c r="C60" s="23"/>
       <c r="D60" s="24"/>
     </row>
-    <row r="61" spans="2:5">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" s="6" t="s">
         <v>4</v>
       </c>
@@ -1579,7 +1587,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="2:5">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" s="9" t="s">
         <v>7</v>
       </c>
@@ -1593,7 +1601,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="2:5">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" s="9" t="s">
         <v>10</v>
       </c>
@@ -1607,7 +1615,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="2:5">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" s="9" t="s">
         <v>7</v>
       </c>
@@ -1617,7 +1625,7 @@
       <c r="D64" s="9"/>
       <c r="E64" s="19"/>
     </row>
-    <row r="65" spans="2:5">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B65" s="9" t="s">
         <v>10</v>
       </c>
@@ -1627,7 +1635,7 @@
       <c r="D65" s="9"/>
       <c r="E65" s="19"/>
     </row>
-    <row r="66" spans="2:5">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B66" s="17" t="s">
         <v>43</v>
       </c>
@@ -1635,7 +1643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:5">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B67" s="17" t="s">
         <v>44</v>
       </c>
@@ -1667,327 +1675,327 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="145.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="str">
         <f>"&lt;forecast seriesName="&amp;CHAR(34)&amp;Schedules!D2&amp;CHAR(34)&amp;"&gt;"</f>
         <v>&lt;forecast seriesName="Mening"&gt;</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="MCV4" vaccineIds="183, 184, 198"/&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B5&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C5&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="MPSV4" vaccineIds="182"/&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B6&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C6&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Menveo" vaccineIds="198"/&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B7&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C7&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Menactra" vaccineIds="183"/&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B25&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C25&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D25&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E24&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="A1" dose="1" indication="BIRTH" label="1st"&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C47&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C46&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="1"/&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C28&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D28&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E28&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="8 weeks" interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C29&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D29&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E29&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C30&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D30&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E30&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="11 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C31&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D31&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E31&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="13 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C32&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D32&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E32&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="22 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D33&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E33&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D34&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B37&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C37&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D37&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E37&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Menactra" schedule="INVALID" age="9 months -4 days" reason="Menactra not licensed before 9 months."/&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B38&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C38&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D38&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E38&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="INVALID" age="2 years -4 days" reason="MPSV4 not licensed before 2 years."/&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B39&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C39&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D39&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E39&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Menveo" schedule="INVALID" age="2 months -4 days" reason="Menveo not licensed before 2 months."/&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B40&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C40&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D40&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E40&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="A1" age="10 years" reason="Received dose of MCV4 before 10 years, not counting towards completion."/&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B41&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C41&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D41&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E41&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="A1" age="10 years" reason="Received dose of MPSV4 before 10 years, not counting towards completion."/&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B42&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C42&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D42&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E42&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="A2" age="16 years -4 days" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B43&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C43&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D43&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E43&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="A2" age="16 years -4 days" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B44&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C44&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D44&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E44&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="COMPLETE" age="" reason="Only one dose needed if administered after 15 years of age."/&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B45&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C45&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D45&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E45&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="COMPLETE" age="" reason="Only one dose needed if administered after 15 years of age."/&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B50&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C50&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D50&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E49&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="A2" dose="2" indication="" label="2nd"&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C67&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C66&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C53&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D53&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E53&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="16 years" interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C54&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D54&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E54&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C55&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D55&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E55&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="16 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C56&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D56&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E56&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="17 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="21" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C57&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D57&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E57&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;finished age="22 years" interval="" grace=""/&gt;</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
+        <v xml:space="preserve">    &lt;finished age="19 years" interval="" grace=""/&gt;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D58&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E58&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="21" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D59&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B62&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C62&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D62&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E62&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="A2" age="16 years -4 days" reason="Received dose before 16 years of age, not counting towards completion."/&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B63&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C63&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D63&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E63&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="A2" age="16 years -4 days" reason="Received dose before 16 years of age, not counting towards completion."/&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B64&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C64&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D64&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E64&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B65&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C65&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D65&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E65&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="20"/>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="21"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="21"/>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="21"/>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="21"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="21"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="21"/>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="21"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="21"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="21"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="21"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="21"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="21"/>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="20"/>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="21"/>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="21"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="21"/>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="21"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="21"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="21"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="21"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="21"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="21"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="21"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="21"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="20"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update HepB and Mening (MCV4) schedules: - Adjusted finish age to 19 years for 1st dose of MCV4 (this change was already made for the booster dose) - Added multiple HepB formulations to the list of valid doses for the HepB birth dose
Update version to 3.14.07
</commit_message>
<xml_diff>
--- a/schedules/Mening.xlsx
+++ b/schedules/Mening.xlsx
@@ -5,26 +5,26 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCHWorkspaceJava6\forecaster\schedules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCHWorkspaceJava6\fv\schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="0" windowWidth="19335" windowHeight="18585" tabRatio="396"/>
+    <workbookView xWindow="2685" yWindow="0" windowWidth="19335" windowHeight="18585" tabRatio="396" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
     <sheet name="XML" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Excel_BuiltIn_Print_Area_1">Schedules!$A$1:$K$47</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$K$70</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_1">Schedules!$A$1:$K$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$K$68</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="63">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -229,9 +229,6 @@
     <t>9 months -4 days</t>
   </si>
   <si>
-    <t>22 years</t>
-  </si>
-  <si>
     <t>2 months -4 days</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   </si>
   <si>
     <t>19 years</t>
+  </si>
+  <si>
+    <t>MPSV4 does not count for 16 year old dose</t>
   </si>
 </sst>
 </file>
@@ -967,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J67"/>
+  <dimension ref="B1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1271,7 +1271,7 @@
         <v>32</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -1339,7 +1339,7 @@
         <v>42</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>50</v>
@@ -1353,7 +1353,7 @@
         <v>42</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>55</v>
@@ -1406,10 +1406,10 @@
       <c r="C43" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D43" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E43" s="19"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="19" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" s="9" t="s">
@@ -1424,238 +1424,214 @@
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B45" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D45" s="9"/>
-      <c r="E45" s="19" t="s">
-        <v>41</v>
+      <c r="B45" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C46" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B47" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B49" s="5" t="s">
+    <row r="48" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B48" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C48" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D48" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E49" s="14" t="s">
+      <c r="E48" s="14" t="s">
         <v>45</v>
       </c>
     </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" s="15">
+        <v>2</v>
+      </c>
+      <c r="D49" s="15"/>
+    </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B50" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" s="15">
-        <v>2</v>
-      </c>
-      <c r="D50" s="15"/>
+      <c r="B50" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="24"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B51" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="24"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B52" s="16"/>
-      <c r="C52" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>24</v>
+      <c r="B52" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>27</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C54" s="9"/>
+        <v>29</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" s="17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
+        <v>33</v>
+      </c>
+      <c r="C57" s="18"/>
+      <c r="D57" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C58" s="18"/>
-      <c r="D58" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>27</v>
-      </c>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B59" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C59" s="18"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
+      <c r="B59" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C59" s="23"/>
+      <c r="D59" s="24"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B60" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C60" s="23"/>
-      <c r="D60" s="24"/>
+      <c r="B60" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B61" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>37</v>
+      <c r="B61" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" s="9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D62" s="9" t="s">
-        <v>57</v>
-      </c>
+      <c r="D62" s="9"/>
       <c r="E62" s="19" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" s="9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E63" s="19" t="s">
-        <v>54</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D63" s="9"/>
+      <c r="E63" s="19"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B64" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D64" s="9"/>
-      <c r="E64" s="19"/>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B65" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D65" s="9"/>
-      <c r="E65" s="19"/>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B66" s="17" t="s">
+      <c r="B64" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C66" s="9">
+      <c r="C64" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B67" s="17" t="s">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B65" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C67" s="9">
+      <c r="C65" s="9">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="5">
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B59:D59"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="B35:D35"/>
@@ -1676,15 +1652,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A65"/>
+  <dimension ref="A1:A63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="145.85546875" customWidth="1"/>
+    <col min="1" max="1" width="137.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -1725,7 +1701,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C47&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C46&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C46&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C45&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="1"/&gt;</v>
       </c>
     </row>
@@ -1756,7 +1732,7 @@
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C32&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D32&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E32&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;finished age="22 years" interval="" grace=""/&gt;</v>
+        <v xml:space="preserve">    &lt;finished age="19 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
@@ -1810,7 +1786,7 @@
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B43&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C43&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D43&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E43&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="A2" age="16 years -4 days" reason=""/&gt;</v>
+        <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="A2" age="" reason="MPSV4 does not count for 16 year old dose"/&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
@@ -1821,107 +1797,101 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B45&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C45&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D45&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E45&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="COMPLETE" age="" reason="Only one dose needed if administered after 15 years of age."/&gt;</v>
+        <f>"  &lt;/schedule&gt;"</f>
+        <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="str">
-        <f>"  &lt;/schedule&gt;"</f>
-        <v xml:space="preserve">  &lt;/schedule&gt;</v>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B49&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C49&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D49&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E48&amp;CHAR(34)&amp;"&gt;"</f>
+        <v xml:space="preserve">  &lt;schedule scheduleName="A2" dose="2" indication="" label="2nd"&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="21" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B50&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C50&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D50&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E49&amp;CHAR(34)&amp;"&gt;"</f>
-        <v xml:space="preserve">  &lt;schedule scheduleName="A2" dose="2" indication="" label="2nd"&gt;</v>
+      <c r="A25" s="20" t="str">
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C65&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C64&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C67&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C66&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
+      <c r="A26" s="21" t="str">
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C52&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D52&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E52&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;valid age="16 years" interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C53&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D53&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E53&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;valid age="16 years" interval="8 weeks" grace="4 days"/&gt;</v>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C53&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D53&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E53&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C54&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D54&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E54&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C54&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D54&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E54&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;due age="16 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C55&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D55&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E55&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;due age="16 years" interval="" grace=""/&gt;</v>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C55&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D55&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E55&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;overdue age="17 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C56&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D56&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E56&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;overdue age="17 years" interval="" grace=""/&gt;</v>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C56&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D56&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E56&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;finished age="19 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="21" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C57&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D57&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E57&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;finished age="19 years" interval="" grace=""/&gt;</v>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D57&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E57&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D58&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E58&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 days"/&gt;</v>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D58&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="21" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D59&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B61&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C61&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D61&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E61&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="A2" age="16 years -4 days" reason="Received dose before 16 years of age, not counting towards completion."/&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B62&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C62&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D62&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E62&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="A2" age="16 years -4 days" reason="Received dose before 16 years of age, not counting towards completion."/&gt;</v>
+        <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="A2" age="" reason="MPSV4 does not count for 16 year old dose"/&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B63&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C63&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D63&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E63&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="A2" age="16 years -4 days" reason="Received dose before 16 years of age, not counting towards completion."/&gt;</v>
+        <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B64&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C64&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D64&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E64&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="MCV4" schedule="COMPLETE" age="" reason=""/&gt;</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B65&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C65&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D65&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E65&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="MPSV4" schedule="COMPLETE" age="" reason=""/&gt;</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="21" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="20"/>
+    </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="21" t="s">
-        <v>56</v>
-      </c>
+      <c r="A39" s="21"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="20"/>
+      <c r="A40" s="21"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="21"/>
@@ -1954,13 +1924,13 @@
       <c r="A50" s="21"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="21"/>
+      <c r="A51" s="20"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="21"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="20"/>
+      <c r="A53" s="21"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="21"/>
@@ -1990,13 +1960,7 @@
       <c r="A62" s="21"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="21"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="21"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="20"/>
+      <c r="A63" s="20"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>